<commit_message>
experiment Update. correction:sse to long type
</commit_message>
<xml_diff>
--- a/experiment.xlsx
+++ b/experiment.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="send-v" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="74">
   <si>
     <t>parallelism</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -150,6 +150,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>main.java.calculation.exact.sendcoef.BaselineImpl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>main.java.calculation.exact.sendv.BaselineFreqImpl</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -266,6 +270,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>basics</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>improveds</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -299,6 +307,18 @@
   </si>
   <si>
     <t>twos</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sendcoef</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8m22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11m8s</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -589,6 +609,55 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>169853</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>89771</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>158095</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E5F2394-2ABD-40D4-A1AA-1EF62E09C00B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1236653"/>
+          <a:ext cx="7468471" cy="2655242"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>31750</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -853,7 +922,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1122,7 +1191,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1204,6 +1273,94 @@
         <a:xfrm>
           <a:off x="0" y="5710358"/>
           <a:ext cx="7891245" cy="1915553"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>96026</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>9081</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55DCE03A-CB2B-47D0-9F43-0CDEFE017182}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="9086850"/>
+          <a:ext cx="10116326" cy="2479231"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>37211</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>477602</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>170960</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1FB2A49-A8EE-44A6-BAEF-6A0B86669B29}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="57150" y="13194411"/>
+          <a:ext cx="7138752" cy="1911749"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1480,8 +1637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="G94" sqref="G94"/>
+    <sheetView topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1498,7 +1655,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D1" t="s">
         <v>18</v>
@@ -1528,7 +1685,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1555,7 +1712,7 @@
         <v>14</v>
       </c>
       <c r="B7">
-        <v>1741399872</v>
+        <v>700062878179</v>
       </c>
       <c r="E7" t="str">
         <f>"/share/flink/tmp/freqs/dataset245freq.txt /share/flink/tmp/freqs/"&amp;TEXT(C1,0)&amp;"k"&amp;TEXT(B3,0)&amp;"e4coeffreq.txt  /share/flink/tmp/"&amp;TEXT(C1,0)&amp;"k"&amp;TEXT(B3,0)&amp;"sse.txt "</f>
@@ -1570,7 +1727,7 @@
         <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D25" t="s">
         <v>18</v>
@@ -1584,7 +1741,7 @@
         <v>40</v>
       </c>
       <c r="D26" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1600,7 +1757,7 @@
         <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1608,7 +1765,7 @@
         <v>15</v>
       </c>
       <c r="B29" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1616,7 +1773,7 @@
         <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E30" t="s">
         <v>25</v>
@@ -1626,6 +1783,9 @@
       <c r="A31" t="s">
         <v>14</v>
       </c>
+      <c r="B31">
+        <v>583796393311</v>
+      </c>
       <c r="E31" t="str">
         <f>"/share/flink/tmp/freqs/dataset245freq.txt /share/flink/tmp/freqs/"&amp;TEXT(C25,0)&amp;"k"&amp;TEXT(B27,0)&amp;"coeffreq.txt  /share/flink/tmp/"&amp;TEXT(C25,0)&amp;"k"&amp;TEXT(B27,0)&amp;"sse.txt "</f>
         <v xml:space="preserve">/share/flink/tmp/freqs/dataset245freq.txt /share/flink/tmp/freqs/sendvk20coeffreq.txt  /share/flink/tmp/sendvk20sse.txt </v>
@@ -1639,7 +1799,7 @@
         <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D48" t="s">
         <v>18</v>
@@ -1653,7 +1813,7 @@
         <v>40</v>
       </c>
       <c r="D49" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -1669,7 +1829,7 @@
         <v>2</v>
       </c>
       <c r="B51" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -1677,7 +1837,7 @@
         <v>15</v>
       </c>
       <c r="B52" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -1685,7 +1845,7 @@
         <v>10</v>
       </c>
       <c r="B53" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E53" t="s">
         <v>25</v>
@@ -1696,7 +1856,7 @@
         <v>14</v>
       </c>
       <c r="B54">
-        <v>988476352</v>
+        <v>572219126720</v>
       </c>
       <c r="E54" t="str">
         <f>"/share/flink/tmp/freqs/dataset245freq.txt /share/flink/tmp/freqs/"&amp;TEXT(C48,0)&amp;"k"&amp;TEXT(B50,0)&amp;"coeffreq.txt  /share/flink/tmp/"&amp;TEXT(C48,0)&amp;"k"&amp;TEXT(B50,0)&amp;"sse.txt "</f>
@@ -1711,7 +1871,7 @@
         <v>4</v>
       </c>
       <c r="C69" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D69" t="s">
         <v>18</v>
@@ -1725,7 +1885,7 @@
         <v>40</v>
       </c>
       <c r="D70" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
@@ -1741,7 +1901,7 @@
         <v>2</v>
       </c>
       <c r="B72" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
@@ -1749,7 +1909,7 @@
         <v>15</v>
       </c>
       <c r="B73" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
@@ -1757,7 +1917,7 @@
         <v>10</v>
       </c>
       <c r="B74" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E74" t="s">
         <v>25</v>
@@ -1768,7 +1928,7 @@
         <v>14</v>
       </c>
       <c r="B75">
-        <v>956279786</v>
+        <v>550712093674</v>
       </c>
       <c r="E75" t="str">
         <f>"/share/flink/tmp/freqs/dataset245freq.txt /share/flink/tmp/freqs/"&amp;TEXT(C69,0)&amp;"k"&amp;TEXT(B71,0)&amp;"coeffreq.txt  /share/flink/tmp/"&amp;TEXT(C69,0)&amp;"k"&amp;TEXT(B71,0)&amp;"sse.txt "</f>
@@ -1783,7 +1943,7 @@
         <v>5</v>
       </c>
       <c r="C91" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D91" t="s">
         <v>18</v>
@@ -1797,7 +1957,7 @@
         <v>40</v>
       </c>
       <c r="D92" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
@@ -1813,7 +1973,7 @@
         <v>2</v>
       </c>
       <c r="B94" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
@@ -1821,7 +1981,7 @@
         <v>15</v>
       </c>
       <c r="B95" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
@@ -1829,7 +1989,7 @@
         <v>10</v>
       </c>
       <c r="B96" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E96" t="s">
         <v>25</v>
@@ -1838,6 +1998,9 @@
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>14</v>
+      </c>
+      <c r="B97">
+        <v>544444457240</v>
       </c>
       <c r="E97" t="str">
         <f>"/share/flink/tmp/freqs/dataset245freq.txt /share/flink/tmp/freqs/"&amp;TEXT(C91,0)&amp;"k"&amp;TEXT(B93,0)&amp;"coeffreq.txt  /share/flink/tmp/"&amp;TEXT(C91,0)&amp;"k"&amp;TEXT(B93,0)&amp;"sse.txt "</f>
@@ -1856,7 +2019,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1870,7 +2033,7 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D1" t="s">
         <v>18</v>
@@ -1906,7 +2069,7 @@
         <v>15</v>
       </c>
       <c r="B5" t="str">
-        <f>"/share/flink/tmp/dataset245.txt 50  /share/flink/tmp/"&amp;TEXT(C1,0)&amp;"k"&amp;TEXT(B3,0)&amp;"coef.txt"</f>
+        <f>"/share/flink/tmp/dataset245.txt "&amp;TEXT(B3,0)&amp;"  /share/flink/tmp/"&amp;TEXT(C1,0)&amp;"k"&amp;TEXT(B3,0)&amp;"coef.txt"</f>
         <v>/share/flink/tmp/dataset245.txt 50  /share/flink/tmp/sendvk50coef.txt</v>
       </c>
     </row>
@@ -1932,7 +2095,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D10" t="s">
         <v>18</v>
@@ -1947,7 +2110,7 @@
       </c>
       <c r="D11" t="str">
         <f>"java -jar -Xmx40000m wavelet.jar /share/flink/tmp/"&amp;TEXT(C10,0)&amp;"k"&amp;TEXT(B12,0)&amp;"e"&amp;TEXT(B13,0)&amp;"coef.txt   /share/flink/tmp/freqs/"&amp;TEXT(C10,0)&amp;"k"&amp;TEXT(B12,0)&amp;"e"&amp;TEXT(B13,0)&amp;"coeffreq.txt"</f>
-        <v>java -jar -Xmx40000m wavelet.jar /share/flink/tmp/improvedsk20e4coef.txt   /share/flink/tmp/freqs/improvedsk20e4coeffreq.txt</v>
+        <v>java -jar -Xmx40000m wavelet.jar /share/flink/tmp/improvedsk30e4coef.txt   /share/flink/tmp/freqs/improvedsk30e4coeffreq.txt</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -1955,12 +2118,12 @@
         <v>4</v>
       </c>
       <c r="B12">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -1981,7 +2144,7 @@
       </c>
       <c r="B15" t="str">
         <f>"/share/flink/tmp/dataset245.txt "&amp;TEXT(B12,0)&amp;"  "&amp;TEXT(POWER(0.1,B13),"0.00000")&amp;" /share/flink/tmp/"&amp;TEXT(C10,0)&amp;"k"&amp;TEXT(B12,0)&amp;"e"&amp;TEXT(B13,0)&amp;"coef.txt"</f>
-        <v>/share/flink/tmp/dataset245.txt 20  0.00010 /share/flink/tmp/improvedsk20e4coef.txt</v>
+        <v>/share/flink/tmp/dataset245.txt 30  0.00010 /share/flink/tmp/improvedsk30e4coef.txt</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -1998,7 +2161,7 @@
       </c>
       <c r="E17" t="str">
         <f>"/share/flink/tmp/freqs/dataset245freq.txt /share/flink/tmp/freqs/"&amp;TEXT(C10,0)&amp;"k"&amp;TEXT(B12,0)&amp;"e"&amp;TEXT(B13,0)&amp;"coeffreq.txt  /share/flink/tmp/"&amp;TEXT(C10,0)&amp;"k"&amp;TEXT(B12,0)&amp;"e"&amp;TEXT(B13,0)&amp;"sse.txt "</f>
-        <v xml:space="preserve">/share/flink/tmp/freqs/dataset245freq.txt /share/flink/tmp/freqs/improvedsk20e4coeffreq.txt  /share/flink/tmp/improvedsk20e4sse.txt </v>
+        <v xml:space="preserve">/share/flink/tmp/freqs/dataset245freq.txt /share/flink/tmp/freqs/improvedsk30e4coeffreq.txt  /share/flink/tmp/improvedsk30e4sse.txt </v>
       </c>
     </row>
   </sheetData>
@@ -2009,10 +2172,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD8"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2020,18 +2183,88 @@
     <col min="1" max="1" width="31.58203125" customWidth="1"/>
     <col min="2" max="2" width="13.25" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>40</v>
+      </c>
+      <c r="D2" t="str">
+        <f>"java -jar -Xmx40000m wavelet.jar /share/flink/tmp/"&amp;TEXT(C1,0)&amp;"k"&amp;TEXT(B3,0)&amp;"coef.txt   /share/flink/tmp/freqs/"&amp;TEXT(C1,0)&amp;"k"&amp;TEXT(B3,0)&amp;"coeffreq.txt"</f>
+        <v>java -jar -Xmx40000m wavelet.jar /share/flink/tmp/sendcoefk10coef.txt   /share/flink/tmp/freqs/sendcoefk10coeffreq.txt</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="str">
+        <f>"/share/flink/tmp/dataset245.txt "&amp;TEXT(B3,0)&amp;"  /share/flink/tmp/"&amp;TEXT(C1,0)&amp;"k"&amp;TEXT(B3,0)&amp;"coef.txt 2"</f>
+        <v>/share/flink/tmp/dataset245.txt 10  /share/flink/tmp/sendcoefk10coef.txt 2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="str">
+        <f>"/share/flink/tmp/freqs/dataset245freq.txt /share/flink/tmp/freqs/"&amp;TEXT(C1,0)&amp;"k"&amp;TEXT(B3,0)&amp;"coeffreq.txt  /share/flink/tmp/"&amp;TEXT(C1,0)&amp;"k"&amp;TEXT(B3,0)&amp;"sse.txt "</f>
+        <v xml:space="preserve">/share/flink/tmp/freqs/dataset245freq.txt /share/flink/tmp/freqs/sendcoefk10coeffreq.txt  /share/flink/tmp/sendcoefk10sse.txt </v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E91"/>
+  <dimension ref="A1:E111"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+    <sheetView topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2109,9 +2342,6 @@
       <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B8">
-        <v>1741399872</v>
-      </c>
       <c r="D8" t="s">
         <v>24</v>
       </c>
@@ -2143,7 +2373,7 @@
         <v>20</v>
       </c>
       <c r="D24" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -2167,7 +2397,7 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -2175,7 +2405,7 @@
         <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D28" t="s">
         <v>25</v>
@@ -2186,7 +2416,7 @@
         <v>14</v>
       </c>
       <c r="D29" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -2216,7 +2446,7 @@
         <v>30</v>
       </c>
       <c r="D45" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -2240,7 +2470,7 @@
         <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -2248,7 +2478,7 @@
         <v>10</v>
       </c>
       <c r="B49" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D49" t="s">
         <v>25</v>
@@ -2259,7 +2489,7 @@
         <v>14</v>
       </c>
       <c r="D50" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
@@ -2289,7 +2519,7 @@
         <v>40</v>
       </c>
       <c r="D67" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
@@ -2313,7 +2543,7 @@
         <v>1</v>
       </c>
       <c r="B70" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
@@ -2321,10 +2551,10 @@
         <v>10</v>
       </c>
       <c r="B71" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C71" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E71" t="s">
         <v>25</v>
@@ -2335,7 +2565,7 @@
         <v>14</v>
       </c>
       <c r="E72" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
@@ -2365,7 +2595,7 @@
         <v>50</v>
       </c>
       <c r="D86" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
@@ -2389,7 +2619,7 @@
         <v>1</v>
       </c>
       <c r="B89" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
@@ -2405,10 +2635,87 @@
         <v>14</v>
       </c>
       <c r="B91" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E91" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>9</v>
+      </c>
+      <c r="B104">
+        <v>6</v>
+      </c>
+      <c r="C104" t="s">
+        <v>61</v>
+      </c>
+      <c r="D104" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>0</v>
+      </c>
+      <c r="B105">
+        <v>40</v>
+      </c>
+      <c r="D105" t="str">
+        <f>"java -jar -Xmx40000m wavelet.jar /share/flink/tmp/"&amp;TEXT(C104,0)&amp;"k"&amp;TEXT(B106,0)&amp;"e"&amp;TEXT(B107,0)&amp;"coef.txt   /share/flink/tmp/freqs/"&amp;TEXT(C104,0)&amp;"k"&amp;TEXT(B106,0)&amp;"e"&amp;TEXT(B107,0)&amp;"coeffreq.txt"</f>
+        <v>java -jar -Xmx40000m wavelet.jar /share/flink/tmp/basicsk30e1coef.txt   /share/flink/tmp/freqs/basicsk30e1coeffreq.txt</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>4</v>
+      </c>
+      <c r="B106">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>60</v>
+      </c>
+      <c r="B107">
+        <v>1</v>
+      </c>
+      <c r="C107">
+        <f>POWER(0.1,B107)</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>1</v>
+      </c>
+      <c r="B109" t="str">
+        <f>"/share/flink/tmp/dataset245.txt "&amp;TEXT(B106,0)&amp;"  "&amp;TEXT(POWER(0.1,B107),"0.00000")&amp;" /share/flink/tmp/"&amp;TEXT(C104,0)&amp;"k"&amp;TEXT(B106,0)&amp;"e"&amp;TEXT(B107,0)&amp;"coef.txt"</f>
+        <v>/share/flink/tmp/dataset245.txt 30  0.10000 /share/flink/tmp/basicsk30e1coef.txt</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>10</v>
+      </c>
+      <c r="E110" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>14</v>
+      </c>
+      <c r="E111" t="str">
+        <f>"/share/flink/tmp/freqs/dataset245freq.txt /share/flink/tmp/freqs/"&amp;TEXT(C104,0)&amp;"k"&amp;TEXT(B106,0)&amp;"e"&amp;TEXT(B107,0)&amp;"coeffreq.txt  /share/flink/tmp/"&amp;TEXT(C104,0)&amp;"k"&amp;TEXT(B106,0)&amp;"e"&amp;TEXT(B107,0)&amp;"sse.txt "</f>
+        <v xml:space="preserve">/share/flink/tmp/freqs/dataset245freq.txt /share/flink/tmp/freqs/basicsk30e1coeffreq.txt  /share/flink/tmp/basicsk30e1sse.txt </v>
       </c>
     </row>
   </sheetData>
@@ -2420,10 +2727,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E88"/>
+  <dimension ref="A1:E109"/>
   <sheetViews>
-    <sheetView topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81:XFD88"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2441,7 +2748,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -2468,7 +2775,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -2502,7 +2809,7 @@
         <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E7" t="s">
         <v>25</v>
@@ -2525,7 +2832,7 @@
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D21" t="s">
         <v>18</v>
@@ -2553,7 +2860,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B24">
         <v>4</v>
@@ -2585,7 +2892,7 @@
         <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E27" t="s">
         <v>25</v>
@@ -2608,7 +2915,7 @@
         <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D41" t="s">
         <v>18</v>
@@ -2636,7 +2943,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B44">
         <v>4</v>
@@ -2668,7 +2975,7 @@
         <v>10</v>
       </c>
       <c r="B47" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E47" t="s">
         <v>25</v>
@@ -2691,7 +2998,7 @@
         <v>4</v>
       </c>
       <c r="C61" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D61" t="s">
         <v>18</v>
@@ -2719,7 +3026,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B64">
         <v>4</v>
@@ -2751,7 +3058,7 @@
         <v>10</v>
       </c>
       <c r="B67" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E67" t="s">
         <v>25</v>
@@ -2774,7 +3081,7 @@
         <v>5</v>
       </c>
       <c r="C81" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D81" t="s">
         <v>18</v>
@@ -2802,7 +3109,7 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B84">
         <v>4</v>
@@ -2834,7 +3141,7 @@
         <v>10</v>
       </c>
       <c r="B87" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E87" t="s">
         <v>25</v>
@@ -2847,6 +3154,83 @@
       <c r="E88" t="str">
         <f>"/share/flink/tmp/freqs/dataset245freq.txt /share/flink/tmp/freqs/"&amp;TEXT(C81,0)&amp;"k"&amp;TEXT(B83,0)&amp;"e"&amp;TEXT(B84,0)&amp;"coeffreq.txt  /share/flink/tmp/"&amp;TEXT(C81,0)&amp;"k"&amp;TEXT(B83,0)&amp;"e"&amp;TEXT(B84,0)&amp;"sse.txt "</f>
         <v xml:space="preserve">/share/flink/tmp/freqs/dataset245freq.txt /share/flink/tmp/freqs/improvedsk50e4coeffreq.txt  /share/flink/tmp/improvedsk50e4sse.txt </v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>9</v>
+      </c>
+      <c r="B102">
+        <v>6</v>
+      </c>
+      <c r="C102" t="s">
+        <v>62</v>
+      </c>
+      <c r="D102" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>0</v>
+      </c>
+      <c r="B103">
+        <v>40</v>
+      </c>
+      <c r="D103" t="str">
+        <f>"java -jar -Xmx40000m wavelet.jar /share/flink/tmp/"&amp;TEXT(C102,0)&amp;"k"&amp;TEXT(B104,0)&amp;"e"&amp;TEXT(B105,0)&amp;"coef.txt   /share/flink/tmp/freqs/"&amp;TEXT(C102,0)&amp;"k"&amp;TEXT(B104,0)&amp;"e"&amp;TEXT(B105,0)&amp;"coeffreq.txt"</f>
+        <v>java -jar -Xmx40000m wavelet.jar /share/flink/tmp/improvedsk30e1coef.txt   /share/flink/tmp/freqs/improvedsk30e1coeffreq.txt</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>4</v>
+      </c>
+      <c r="B104">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>60</v>
+      </c>
+      <c r="B105">
+        <v>1</v>
+      </c>
+      <c r="C105">
+        <f>POWER(0.1,B105)</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>1</v>
+      </c>
+      <c r="B107" t="str">
+        <f>"/share/flink/tmp/dataset245.txt "&amp;TEXT(B104,0)&amp;"  "&amp;TEXT(POWER(0.1,B105),"0.00000")&amp;" /share/flink/tmp/"&amp;TEXT(C102,0)&amp;"k"&amp;TEXT(B104,0)&amp;"e"&amp;TEXT(B105,0)&amp;"coef.txt"</f>
+        <v>/share/flink/tmp/dataset245.txt 30  0.10000 /share/flink/tmp/improvedsk30e1coef.txt</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>10</v>
+      </c>
+      <c r="E108" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>14</v>
+      </c>
+      <c r="E109" t="str">
+        <f>"/share/flink/tmp/freqs/dataset245freq.txt /share/flink/tmp/freqs/"&amp;TEXT(C102,0)&amp;"k"&amp;TEXT(B104,0)&amp;"e"&amp;TEXT(B105,0)&amp;"coeffreq.txt  /share/flink/tmp/"&amp;TEXT(C102,0)&amp;"k"&amp;TEXT(B104,0)&amp;"e"&amp;TEXT(B105,0)&amp;"sse.txt "</f>
+        <v xml:space="preserve">/share/flink/tmp/freqs/dataset245freq.txt /share/flink/tmp/freqs/improvedsk30e1coeffreq.txt  /share/flink/tmp/improvedsk30e1sse.txt </v>
       </c>
     </row>
   </sheetData>
@@ -2858,10 +3242,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E93"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2870,15 +3254,18 @@
     <col min="2" max="2" width="13.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
       <c r="B1">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2889,7 +3276,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2900,7 +3287,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -2908,15 +3295,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <f>POWER(0.1,B5)</f>
+        <v>1.0000000000000005E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -2924,7 +3315,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -2932,17 +3323,27 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
+      </c>
+      <c r="B9">
+        <v>700911821068</v>
+      </c>
+      <c r="E9" t="str">
+        <f>"/share/flink/tmp/freqs/dataset245freq.txt /share/flink/tmp/freqs/"&amp;TEXT(C1,0)&amp;"k"&amp;TEXT(B3,0)&amp;"e"&amp;TEXT(B5,0)&amp;"coeffreq.txt  /share/flink/tmp/"&amp;TEXT(C1,0)&amp;"k"&amp;TEXT(B3,0)&amp;"e"&amp;TEXT(B5,0)&amp;"sse.txt "</f>
+        <v xml:space="preserve">/share/flink/tmp/freqs/dataset245freq.txt /share/flink/tmp/freqs/twosk10e4coeffreq.txt  /share/flink/tmp/twosk10e4sse.txt </v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -2953,7 +3354,7 @@
         <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D25" t="s">
         <v>18</v>
@@ -2981,7 +3382,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B28">
         <v>4</v>
@@ -3013,7 +3414,7 @@
         <v>10</v>
       </c>
       <c r="B31" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E31" t="s">
         <v>25</v>
@@ -3036,7 +3437,7 @@
         <v>3</v>
       </c>
       <c r="C44" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D44" t="s">
         <v>18</v>
@@ -3064,7 +3465,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B47">
         <v>4</v>
@@ -3095,6 +3496,9 @@
       <c r="A50" t="s">
         <v>10</v>
       </c>
+      <c r="B50" t="s">
+        <v>72</v>
+      </c>
       <c r="E50" t="s">
         <v>25</v>
       </c>
@@ -3106,6 +3510,169 @@
       <c r="E51" t="str">
         <f>"/share/flink/tmp/freqs/dataset245freq.txt /share/flink/tmp/freqs/"&amp;TEXT(C44,0)&amp;"k"&amp;TEXT(B46,0)&amp;"e"&amp;TEXT(B47,0)&amp;"coeffreq.txt  /share/flink/tmp/"&amp;TEXT(C44,0)&amp;"k"&amp;TEXT(B46,0)&amp;"e"&amp;TEXT(B47,0)&amp;"sse.txt "</f>
         <v xml:space="preserve">/share/flink/tmp/freqs/dataset245freq.txt /share/flink/tmp/freqs/twosk30e4coeffreq.txt  /share/flink/tmp/twosk30e4sse.txt </v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>9</v>
+      </c>
+      <c r="B67">
+        <v>4</v>
+      </c>
+      <c r="C67" t="s">
+        <v>70</v>
+      </c>
+      <c r="D67" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>0</v>
+      </c>
+      <c r="B68">
+        <v>40</v>
+      </c>
+      <c r="D68" t="str">
+        <f>"java -jar -Xmx40000m wavelet.jar /share/flink/tmp/"&amp;TEXT(C67,0)&amp;"k"&amp;TEXT(B69,0)&amp;"e"&amp;TEXT(B70,0)&amp;"coef.txt   /share/flink/tmp/freqs/"&amp;TEXT(C67,0)&amp;"k"&amp;TEXT(B69,0)&amp;"e"&amp;TEXT(B70,0)&amp;"coeffreq.txt"</f>
+        <v>java -jar -Xmx40000m wavelet.jar /share/flink/tmp/twosk40e4coef.txt   /share/flink/tmp/freqs/twosk40e4coeffreq.txt</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>4</v>
+      </c>
+      <c r="B69">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>60</v>
+      </c>
+      <c r="B70">
+        <v>4</v>
+      </c>
+      <c r="C70">
+        <f>POWER(0.1,B70)</f>
+        <v>1.0000000000000005E-4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>2</v>
+      </c>
+      <c r="B71" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>1</v>
+      </c>
+      <c r="B72" t="str">
+        <f>"/share/flink/tmp/dataset245.txt "&amp;TEXT(B69,0)&amp;"  40 "&amp;TEXT(POWER(0.1,B70),"0.00000")&amp;" /share/flink/tmp/"&amp;TEXT(C67,0)&amp;"k"&amp;TEXT(B69,0)&amp;"e"&amp;TEXT(B70,0)&amp;"coef.txt"</f>
+        <v>/share/flink/tmp/dataset245.txt 40  40 0.00010 /share/flink/tmp/twosk40e4coef.txt</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>10</v>
+      </c>
+      <c r="B73" t="s">
+        <v>73</v>
+      </c>
+      <c r="E73" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>14</v>
+      </c>
+      <c r="E74" t="str">
+        <f>"/share/flink/tmp/freqs/dataset245freq.txt /share/flink/tmp/freqs/"&amp;TEXT(C67,0)&amp;"k"&amp;TEXT(B69,0)&amp;"e"&amp;TEXT(B70,0)&amp;"coeffreq.txt  /share/flink/tmp/"&amp;TEXT(C67,0)&amp;"k"&amp;TEXT(B69,0)&amp;"e"&amp;TEXT(B70,0)&amp;"sse.txt "</f>
+        <v xml:space="preserve">/share/flink/tmp/freqs/dataset245freq.txt /share/flink/tmp/freqs/twosk40e4coeffreq.txt  /share/flink/tmp/twosk40e4sse.txt </v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>9</v>
+      </c>
+      <c r="B86">
+        <v>5</v>
+      </c>
+      <c r="C86" t="s">
+        <v>70</v>
+      </c>
+      <c r="D86" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>0</v>
+      </c>
+      <c r="B87">
+        <v>40</v>
+      </c>
+      <c r="D87" t="str">
+        <f>"java -jar -Xmx40000m wavelet.jar /share/flink/tmp/"&amp;TEXT(C86,0)&amp;"k"&amp;TEXT(B88,0)&amp;"e"&amp;TEXT(B89,0)&amp;"coef.txt   /share/flink/tmp/freqs/"&amp;TEXT(C86,0)&amp;"k"&amp;TEXT(B88,0)&amp;"e"&amp;TEXT(B89,0)&amp;"coeffreq.txt"</f>
+        <v>java -jar -Xmx40000m wavelet.jar /share/flink/tmp/twosk50e4coef.txt   /share/flink/tmp/freqs/twosk50e4coeffreq.txt</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>4</v>
+      </c>
+      <c r="B88">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>60</v>
+      </c>
+      <c r="B89">
+        <v>4</v>
+      </c>
+      <c r="C89">
+        <f>POWER(0.1,B89)</f>
+        <v>1.0000000000000005E-4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>2</v>
+      </c>
+      <c r="B90" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>1</v>
+      </c>
+      <c r="B91" t="str">
+        <f>"/share/flink/tmp/dataset245.txt "&amp;TEXT(B88,0)&amp;"  40 "&amp;TEXT(POWER(0.1,B89),"0.00000")&amp;" /share/flink/tmp/"&amp;TEXT(C86,0)&amp;"k"&amp;TEXT(B88,0)&amp;"e"&amp;TEXT(B89,0)&amp;"coef.txt"</f>
+        <v>/share/flink/tmp/dataset245.txt 50  40 0.00010 /share/flink/tmp/twosk50e4coef.txt</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>10</v>
+      </c>
+      <c r="E92" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>14</v>
+      </c>
+      <c r="E93" t="str">
+        <f>"/share/flink/tmp/freqs/dataset245freq.txt /share/flink/tmp/freqs/"&amp;TEXT(C86,0)&amp;"k"&amp;TEXT(B88,0)&amp;"e"&amp;TEXT(B89,0)&amp;"coeffreq.txt  /share/flink/tmp/"&amp;TEXT(C86,0)&amp;"k"&amp;TEXT(B88,0)&amp;"e"&amp;TEXT(B89,0)&amp;"sse.txt "</f>
+        <v xml:space="preserve">/share/flink/tmp/freqs/dataset245freq.txt /share/flink/tmp/freqs/twosk50e4coeffreq.txt  /share/flink/tmp/twosk50e4sse.txt </v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
experiment update, correct ImprovedSample
</commit_message>
<xml_diff>
--- a/experiment.xlsx
+++ b/experiment.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="send-v" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="79">
   <si>
     <t>parallelism</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -130,10 +130,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>8m 27s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>30m</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -286,26 +282,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>6m9s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>10m37s</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>6m5s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6m14s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6m40s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>twos</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -331,6 +311,34 @@
   </si>
   <si>
     <t>6m26s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7m42s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9m18s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9m10s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8m58s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9m2s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8m56s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8m41s</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1097,7 +1105,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="23329895"/>
+          <a:off x="0" y="25641295"/>
           <a:ext cx="8122959" cy="1850604"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1141,7 +1149,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="26697643"/>
+          <a:off x="0" y="29009043"/>
           <a:ext cx="7726124" cy="1934049"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1220,270 +1228,6 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>267497</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>132931</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CC18980-8B5C-4654-8F6A-FF343EE07550}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="1447800"/>
-          <a:ext cx="9062247" cy="2063331"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>6537</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>17200</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>126494</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8DDE2FC-2A14-44CE-8978-C32110476A78}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9137650" y="1428937"/>
-          <a:ext cx="8259500" cy="2253557"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>23894</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>531574</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>31262</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67B396AC-9737-450C-8007-4AE92D6114D6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="5002294"/>
-          <a:ext cx="7345124" cy="1963168"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>166743</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>582378</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>170967</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1282196-C9D4-45DD-85DE-7C915D8BB3B2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="8523343"/>
-          <a:ext cx="8056328" cy="2137824"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>80</xdr:row>
-      <xdr:rowOff>52023</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>379221</xdr:colOff>
-      <xdr:row>91</xdr:row>
-      <xdr:rowOff>120183</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A3BE865-0BCD-40C8-ACFC-200750C62B20}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="12142423"/>
-          <a:ext cx="7853171" cy="2023960"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>100</xdr:row>
-      <xdr:rowOff>10599</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>655397</xdr:colOff>
-      <xdr:row>112</xdr:row>
-      <xdr:rowOff>18605</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE2283B2-FF13-4637-9C14-A62CE617BB3B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="15656999"/>
-          <a:ext cx="8789747" cy="2141606"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
@@ -1508,7 +1252,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1517,6 +1261,270 @@
         <a:xfrm>
           <a:off x="38100" y="152400"/>
           <a:ext cx="13400000" cy="1580952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>177329</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>7674</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>59825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D5D4ACD-E486-481E-91C4-C19BC8F8EA62}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="3555529"/>
+          <a:ext cx="8142024" cy="2193896"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>63666</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>407752</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>20185</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF88A70D-D319-4078-9943-B2EA441740C4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="7175666"/>
+          <a:ext cx="7881702" cy="2090119"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>110412</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>25399</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>68031</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>177324</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02923984-09E9-44C7-B3FB-63D4190037AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="110412" y="10693399"/>
+          <a:ext cx="8091969" cy="2107725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>288581</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{525B0880-0591-4259-BBC0-B7327F01AD4D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="14281150"/>
+          <a:ext cx="8422931" cy="2082800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>48574</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>591888</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>154501</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFEE2D84-6CBC-4477-A492-E261ECD31580}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="17828574"/>
+          <a:ext cx="8726238" cy="2239527"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>18738</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>404502</xdr:colOff>
+      <xdr:row>133</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8BA3611-2936-45B8-B58D-2C84724E1200}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="21532538"/>
+          <a:ext cx="9199252" cy="2286311"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1623,13 +1631,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>63</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>132631</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>96026</xdr:colOff>
-      <xdr:row>77</xdr:row>
-      <xdr:rowOff>9081</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>603250</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>117031</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1652,8 +1660,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="9086850"/>
-          <a:ext cx="10116326" cy="2479231"/>
+          <a:off x="0" y="11334031"/>
+          <a:ext cx="8642350" cy="2118000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2080,7 +2088,7 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" t="s">
         <v>18</v>
@@ -2110,7 +2118,7 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -2126,7 +2134,7 @@
         <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E18" t="s">
         <v>25</v>
@@ -2152,7 +2160,7 @@
         <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D37" t="s">
         <v>18</v>
@@ -2166,7 +2174,7 @@
         <v>40</v>
       </c>
       <c r="D38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -2182,7 +2190,7 @@
         <v>2</v>
       </c>
       <c r="B40" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -2190,7 +2198,7 @@
         <v>15</v>
       </c>
       <c r="B41" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -2198,7 +2206,7 @@
         <v>10</v>
       </c>
       <c r="B42" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E42" t="s">
         <v>25</v>
@@ -2224,7 +2232,7 @@
         <v>3</v>
       </c>
       <c r="C60" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D60" t="s">
         <v>18</v>
@@ -2238,7 +2246,7 @@
         <v>40</v>
       </c>
       <c r="D61" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -2254,7 +2262,7 @@
         <v>2</v>
       </c>
       <c r="B63" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -2262,7 +2270,7 @@
         <v>15</v>
       </c>
       <c r="B64" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
@@ -2270,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="B65" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E65" t="s">
         <v>25</v>
@@ -2296,7 +2304,7 @@
         <v>4</v>
       </c>
       <c r="C81" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D81" t="s">
         <v>18</v>
@@ -2310,7 +2318,7 @@
         <v>40</v>
       </c>
       <c r="D82" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
@@ -2326,7 +2334,7 @@
         <v>2</v>
       </c>
       <c r="B84" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
@@ -2334,7 +2342,7 @@
         <v>15</v>
       </c>
       <c r="B85" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
@@ -2342,7 +2350,7 @@
         <v>10</v>
       </c>
       <c r="B86" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E86" t="s">
         <v>25</v>
@@ -2368,7 +2376,7 @@
         <v>5</v>
       </c>
       <c r="C103" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D103" t="s">
         <v>18</v>
@@ -2382,7 +2390,7 @@
         <v>40</v>
       </c>
       <c r="D104" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
@@ -2398,7 +2406,7 @@
         <v>2</v>
       </c>
       <c r="B106" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
@@ -2406,7 +2414,7 @@
         <v>15</v>
       </c>
       <c r="B107" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
@@ -2414,7 +2422,7 @@
         <v>10</v>
       </c>
       <c r="B108" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E108" t="s">
         <v>25</v>
@@ -2459,7 +2467,7 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
         <v>18</v>
@@ -2521,7 +2529,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D10" t="s">
         <v>18</v>
@@ -2549,7 +2557,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -2616,7 +2624,7 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D13" t="s">
         <v>18</v>
@@ -2647,7 +2655,7 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -2687,8 +2695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A14:E182"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="J124" sqref="J124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2766,6 +2774,9 @@
       <c r="A21" t="s">
         <v>14</v>
       </c>
+      <c r="B21">
+        <v>701201023371</v>
+      </c>
       <c r="D21" t="s">
         <v>24</v>
       </c>
@@ -2797,7 +2808,7 @@
         <v>20</v>
       </c>
       <c r="D37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -2821,7 +2832,7 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -2829,7 +2840,7 @@
         <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D41" t="s">
         <v>25</v>
@@ -2839,8 +2850,11 @@
       <c r="A42" t="s">
         <v>14</v>
       </c>
+      <c r="B42">
+        <v>585087116118</v>
+      </c>
       <c r="D42" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -2870,7 +2884,7 @@
         <v>30</v>
       </c>
       <c r="D58" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -2894,7 +2908,7 @@
         <v>1</v>
       </c>
       <c r="B61" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -2902,7 +2916,7 @@
         <v>10</v>
       </c>
       <c r="B62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D62" t="s">
         <v>25</v>
@@ -2912,8 +2926,11 @@
       <c r="A63" t="s">
         <v>14</v>
       </c>
+      <c r="B63">
+        <v>573524349366</v>
+      </c>
       <c r="D63" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
@@ -2943,7 +2960,7 @@
         <v>40</v>
       </c>
       <c r="D80" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
@@ -2967,7 +2984,7 @@
         <v>1</v>
       </c>
       <c r="B83" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
@@ -2975,10 +2992,10 @@
         <v>10</v>
       </c>
       <c r="B84" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C84" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E84" t="s">
         <v>25</v>
@@ -2989,7 +3006,7 @@
         <v>14</v>
       </c>
       <c r="E85" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
@@ -3019,7 +3036,7 @@
         <v>50</v>
       </c>
       <c r="D99" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
@@ -3043,13 +3060,16 @@
         <v>1</v>
       </c>
       <c r="B102" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>10</v>
       </c>
+      <c r="B103" t="s">
+        <v>64</v>
+      </c>
       <c r="E103" t="s">
         <v>25</v>
       </c>
@@ -3058,11 +3078,8 @@
       <c r="A104" t="s">
         <v>14</v>
       </c>
-      <c r="B104" t="s">
-        <v>66</v>
-      </c>
       <c r="E104" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
@@ -3073,7 +3090,7 @@
         <v>6</v>
       </c>
       <c r="C117" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D117" t="s">
         <v>18</v>
@@ -3101,7 +3118,7 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B120">
         <v>1</v>
@@ -3133,7 +3150,7 @@
         <v>10</v>
       </c>
       <c r="B123" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E123" t="s">
         <v>25</v>
@@ -3156,7 +3173,7 @@
         <v>7</v>
       </c>
       <c r="C137" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D137" t="s">
         <v>18</v>
@@ -3184,7 +3201,7 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B140">
         <v>2</v>
@@ -3216,7 +3233,7 @@
         <v>10</v>
       </c>
       <c r="B143" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E143" t="s">
         <v>25</v>
@@ -3239,7 +3256,7 @@
         <v>8</v>
       </c>
       <c r="C156" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D156" t="s">
         <v>18</v>
@@ -3267,7 +3284,7 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B159">
         <v>3</v>
@@ -3298,6 +3315,9 @@
       <c r="A162" t="s">
         <v>10</v>
       </c>
+      <c r="B162" t="s">
+        <v>72</v>
+      </c>
       <c r="E162" t="s">
         <v>25</v>
       </c>
@@ -3319,7 +3339,7 @@
         <v>9</v>
       </c>
       <c r="C175" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D175" t="s">
         <v>18</v>
@@ -3347,7 +3367,7 @@
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B178">
         <v>5</v>
@@ -3400,10 +3420,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A13:E121"/>
+  <dimension ref="A13:E183"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
+      <selection activeCell="D150" sqref="D150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -3421,7 +3441,7 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -3448,7 +3468,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -3479,10 +3499,7 @@
         <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="E19" t="s">
         <v>25</v>
@@ -3505,7 +3522,7 @@
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D33" t="s">
         <v>18</v>
@@ -3533,7 +3550,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B36">
         <v>4</v>
@@ -3565,7 +3582,7 @@
         <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="E39" t="s">
         <v>25</v>
@@ -3588,7 +3605,7 @@
         <v>3</v>
       </c>
       <c r="C53" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D53" t="s">
         <v>18</v>
@@ -3616,7 +3633,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B56">
         <v>4</v>
@@ -3648,7 +3665,7 @@
         <v>10</v>
       </c>
       <c r="B59" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="E59" t="s">
         <v>25</v>
@@ -3671,7 +3688,7 @@
         <v>4</v>
       </c>
       <c r="C73" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D73" t="s">
         <v>18</v>
@@ -3699,7 +3716,7 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B76">
         <v>4</v>
@@ -3731,7 +3748,7 @@
         <v>10</v>
       </c>
       <c r="B79" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="E79" t="s">
         <v>25</v>
@@ -3754,7 +3771,7 @@
         <v>5</v>
       </c>
       <c r="C93" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D93" t="s">
         <v>18</v>
@@ -3782,7 +3799,7 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B96">
         <v>4</v>
@@ -3814,7 +3831,7 @@
         <v>10</v>
       </c>
       <c r="B99" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="E99" t="s">
         <v>25</v>
@@ -3837,7 +3854,7 @@
         <v>6</v>
       </c>
       <c r="C114" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D114" t="s">
         <v>18</v>
@@ -3865,7 +3882,7 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B117">
         <v>1</v>
@@ -3896,6 +3913,9 @@
       <c r="A120" t="s">
         <v>10</v>
       </c>
+      <c r="B120" t="s">
+        <v>78</v>
+      </c>
       <c r="E120" t="s">
         <v>25</v>
       </c>
@@ -3907,6 +3927,246 @@
       <c r="E121" t="str">
         <f>"/share/flink/tmp/freqs/dataset245freq.txt /share/flink/tmp/freqs/"&amp;TEXT(C114,0)&amp;"k"&amp;TEXT(B116,0)&amp;"e"&amp;TEXT(B117,0)&amp;"coeffreq.txt  /share/flink/tmp/"&amp;TEXT(C114,0)&amp;"k"&amp;TEXT(B116,0)&amp;"e"&amp;TEXT(B117,0)&amp;"sse.txt "</f>
         <v xml:space="preserve">/share/flink/tmp/freqs/dataset245freq.txt /share/flink/tmp/freqs/improvedsk30e1coeffreq.txt  /share/flink/tmp/improvedsk30e1sse.txt </v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>9</v>
+      </c>
+      <c r="B135">
+        <v>7</v>
+      </c>
+      <c r="C135" t="s">
+        <v>61</v>
+      </c>
+      <c r="D135" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>0</v>
+      </c>
+      <c r="B136">
+        <v>40</v>
+      </c>
+      <c r="D136" t="str">
+        <f>"java -jar -Xmx40000m wavelet.jar /share/flink/tmp/"&amp;TEXT(C135,0)&amp;"k"&amp;TEXT(B137,0)&amp;"e"&amp;TEXT(B138,0)&amp;"coef.txt   /share/flink/tmp/freqs/"&amp;TEXT(C135,0)&amp;"k"&amp;TEXT(B137,0)&amp;"e"&amp;TEXT(B138,0)&amp;"coeffreq.txt"</f>
+        <v>java -jar -Xmx40000m wavelet.jar /share/flink/tmp/improvedsk30e2coef.txt   /share/flink/tmp/freqs/improvedsk30e2coeffreq.txt</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>4</v>
+      </c>
+      <c r="B137">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>59</v>
+      </c>
+      <c r="B138">
+        <v>2</v>
+      </c>
+      <c r="C138">
+        <f>POWER(0.1,B138)</f>
+        <v>1.0000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>2</v>
+      </c>
+      <c r="B139" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>1</v>
+      </c>
+      <c r="B140" t="str">
+        <f>"/share/flink/tmp/dataset245.txt "&amp;TEXT(B137,0)&amp;"  "&amp;TEXT(POWER(0.1,B138),"0.00000")&amp;" /share/flink/tmp/"&amp;TEXT(C135,0)&amp;"k"&amp;TEXT(B137,0)&amp;"e"&amp;TEXT(B138,0)&amp;"coef.txt"</f>
+        <v>/share/flink/tmp/dataset245.txt 30  0.01000 /share/flink/tmp/improvedsk30e2coef.txt</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>10</v>
+      </c>
+      <c r="E141" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>14</v>
+      </c>
+      <c r="E142" t="str">
+        <f>"/share/flink/tmp/freqs/dataset245freq.txt /share/flink/tmp/freqs/"&amp;TEXT(C135,0)&amp;"k"&amp;TEXT(B137,0)&amp;"e"&amp;TEXT(B138,0)&amp;"coeffreq.txt  /share/flink/tmp/"&amp;TEXT(C135,0)&amp;"k"&amp;TEXT(B137,0)&amp;"e"&amp;TEXT(B138,0)&amp;"sse.txt "</f>
+        <v xml:space="preserve">/share/flink/tmp/freqs/dataset245freq.txt /share/flink/tmp/freqs/improvedsk30e2coeffreq.txt  /share/flink/tmp/improvedsk30e2sse.txt </v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>9</v>
+      </c>
+      <c r="B156">
+        <v>8</v>
+      </c>
+      <c r="C156" t="s">
+        <v>61</v>
+      </c>
+      <c r="D156" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>0</v>
+      </c>
+      <c r="B157">
+        <v>40</v>
+      </c>
+      <c r="D157" t="str">
+        <f>"java -jar -Xmx40000m wavelet.jar /share/flink/tmp/"&amp;TEXT(C156,0)&amp;"k"&amp;TEXT(B158,0)&amp;"e"&amp;TEXT(B159,0)&amp;"coef.txt   /share/flink/tmp/freqs/"&amp;TEXT(C156,0)&amp;"k"&amp;TEXT(B158,0)&amp;"e"&amp;TEXT(B159,0)&amp;"coeffreq.txt"</f>
+        <v>java -jar -Xmx40000m wavelet.jar /share/flink/tmp/improvedsk30e3coef.txt   /share/flink/tmp/freqs/improvedsk30e3coeffreq.txt</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
+        <v>4</v>
+      </c>
+      <c r="B158">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>59</v>
+      </c>
+      <c r="B159">
+        <v>3</v>
+      </c>
+      <c r="C159">
+        <f>POWER(0.1,B159)</f>
+        <v>1.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>2</v>
+      </c>
+      <c r="B160" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>1</v>
+      </c>
+      <c r="B161" t="str">
+        <f>"/share/flink/tmp/dataset245.txt "&amp;TEXT(B158,0)&amp;"  "&amp;TEXT(POWER(0.1,B159),"0.00000")&amp;" /share/flink/tmp/"&amp;TEXT(C156,0)&amp;"k"&amp;TEXT(B158,0)&amp;"e"&amp;TEXT(B159,0)&amp;"coef.txt"</f>
+        <v>/share/flink/tmp/dataset245.txt 30  0.00100 /share/flink/tmp/improvedsk30e3coef.txt</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>10</v>
+      </c>
+      <c r="E162" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>14</v>
+      </c>
+      <c r="E163" t="str">
+        <f>"/share/flink/tmp/freqs/dataset245freq.txt /share/flink/tmp/freqs/"&amp;TEXT(C156,0)&amp;"k"&amp;TEXT(B158,0)&amp;"e"&amp;TEXT(B159,0)&amp;"coeffreq.txt  /share/flink/tmp/"&amp;TEXT(C156,0)&amp;"k"&amp;TEXT(B158,0)&amp;"e"&amp;TEXT(B159,0)&amp;"sse.txt "</f>
+        <v xml:space="preserve">/share/flink/tmp/freqs/dataset245freq.txt /share/flink/tmp/freqs/improvedsk30e3coeffreq.txt  /share/flink/tmp/improvedsk30e3sse.txt </v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>9</v>
+      </c>
+      <c r="B176">
+        <v>9</v>
+      </c>
+      <c r="C176" t="s">
+        <v>61</v>
+      </c>
+      <c r="D176" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
+        <v>0</v>
+      </c>
+      <c r="B177">
+        <v>40</v>
+      </c>
+      <c r="D177" t="str">
+        <f>"java -jar -Xmx40000m wavelet.jar /share/flink/tmp/"&amp;TEXT(C176,0)&amp;"k"&amp;TEXT(B178,0)&amp;"e"&amp;TEXT(B179,0)&amp;"coef.txt   /share/flink/tmp/freqs/"&amp;TEXT(C176,0)&amp;"k"&amp;TEXT(B178,0)&amp;"e"&amp;TEXT(B179,0)&amp;"coeffreq.txt"</f>
+        <v>java -jar -Xmx40000m wavelet.jar /share/flink/tmp/improvedsk30e5coef.txt   /share/flink/tmp/freqs/improvedsk30e5coeffreq.txt</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>4</v>
+      </c>
+      <c r="B178">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
+        <v>59</v>
+      </c>
+      <c r="B179">
+        <v>5</v>
+      </c>
+      <c r="C179">
+        <f>POWER(0.1,B179)</f>
+        <v>1.0000000000000006E-5</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
+        <v>2</v>
+      </c>
+      <c r="B180" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
+        <v>1</v>
+      </c>
+      <c r="B181" t="str">
+        <f>"/share/flink/tmp/dataset245.txt "&amp;TEXT(B178,0)&amp;"  "&amp;TEXT(POWER(0.1,B179),"0.00000")&amp;" /share/flink/tmp/"&amp;TEXT(C176,0)&amp;"k"&amp;TEXT(B178,0)&amp;"e"&amp;TEXT(B179,0)&amp;"coef.txt"</f>
+        <v>/share/flink/tmp/dataset245.txt 30  0.00001 /share/flink/tmp/improvedsk30e5coef.txt</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A182" t="s">
+        <v>10</v>
+      </c>
+      <c r="E182" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A183" t="s">
+        <v>14</v>
+      </c>
+      <c r="E183" t="str">
+        <f>"/share/flink/tmp/freqs/dataset245freq.txt /share/flink/tmp/freqs/"&amp;TEXT(C176,0)&amp;"k"&amp;TEXT(B178,0)&amp;"e"&amp;TEXT(B179,0)&amp;"coeffreq.txt  /share/flink/tmp/"&amp;TEXT(C176,0)&amp;"k"&amp;TEXT(B178,0)&amp;"e"&amp;TEXT(B179,0)&amp;"sse.txt "</f>
+        <v xml:space="preserve">/share/flink/tmp/freqs/dataset245freq.txt /share/flink/tmp/freqs/improvedsk30e5coeffreq.txt  /share/flink/tmp/improvedsk30e5sse.txt </v>
       </c>
     </row>
   </sheetData>
@@ -3920,8 +4180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A13:E124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="D118" sqref="D118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -3938,7 +4198,7 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -3973,7 +4233,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -3988,7 +4248,7 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -3996,7 +4256,7 @@
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -4004,7 +4264,7 @@
         <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E20" t="s">
         <v>25</v>
@@ -4030,7 +4290,7 @@
         <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D37" t="s">
         <v>18</v>
@@ -4058,7 +4318,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B40">
         <v>4</v>
@@ -4073,7 +4333,7 @@
         <v>2</v>
       </c>
       <c r="B41" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -4090,7 +4350,7 @@
         <v>10</v>
       </c>
       <c r="B43" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E43" t="s">
         <v>25</v>
@@ -4116,7 +4376,7 @@
         <v>3</v>
       </c>
       <c r="C56" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D56" t="s">
         <v>18</v>
@@ -4144,7 +4404,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B59">
         <v>4</v>
@@ -4159,7 +4419,7 @@
         <v>2</v>
       </c>
       <c r="B60" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -4176,7 +4436,7 @@
         <v>10</v>
       </c>
       <c r="B62" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E62" t="s">
         <v>25</v>
@@ -4199,7 +4459,7 @@
         <v>4</v>
       </c>
       <c r="C79" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D79" t="s">
         <v>18</v>
@@ -4227,7 +4487,7 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B82">
         <v>4</v>
@@ -4242,7 +4502,7 @@
         <v>2</v>
       </c>
       <c r="B83" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
@@ -4259,7 +4519,7 @@
         <v>10</v>
       </c>
       <c r="B85" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E85" t="s">
         <v>25</v>
@@ -4282,7 +4542,7 @@
         <v>5</v>
       </c>
       <c r="C98" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D98" t="s">
         <v>18</v>
@@ -4310,7 +4570,7 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B101">
         <v>4</v>
@@ -4325,7 +4585,7 @@
         <v>2</v>
       </c>
       <c r="B102" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
@@ -4342,7 +4602,7 @@
         <v>10</v>
       </c>
       <c r="B104" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E104" t="s">
         <v>25</v>
@@ -4365,7 +4625,7 @@
         <v>6</v>
       </c>
       <c r="C117" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D117" t="s">
         <v>18</v>
@@ -4393,7 +4653,7 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B120">
         <v>1</v>
@@ -4408,7 +4668,7 @@
         <v>2</v>
       </c>
       <c r="B121" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>